<commit_message>
updated for test step execution
</commit_message>
<xml_diff>
--- a/input/input-file.xlsx
+++ b/input/input-file.xlsx
@@ -8,40 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMV\WS\EWS\jtestng\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAAE929-5E61-495A-862C-D937650B26CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDCD16D-9682-46D6-A043-156C60A0E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2AA5BCE-9ACD-4C72-839C-F70134009B4E}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
-    <sheet name="DASHBOARD" sheetId="2" r:id="rId2"/>
-    <sheet name="LOGOUT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
-  <si>
-    <t>SCREEN</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>SELECTOR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>ACTION</t>
   </si>
   <si>
-    <t>INPUT</t>
-  </si>
-  <si>
-    <t>EXPECTED RESULT</t>
-  </si>
-  <si>
     <t>COMMENTS</t>
   </si>
   <si>
@@ -64,81 +47,6 @@
   </si>
   <si>
     <t>CLICK</t>
-  </si>
-  <si>
-    <t>DASHBOARD</t>
-  </si>
-  <si>
-    <t>//img[@class='close-icon ng-star-inserted']</t>
-  </si>
-  <si>
-    <t>//div[@class='welcome-text ng-tns-c3241311687-2']</t>
-  </si>
-  <si>
-    <t>Welcome!</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>Close the popup</t>
-  </si>
-  <si>
-    <t>Check welcome label present</t>
-  </si>
-  <si>
-    <t>//img[@class='Combined-Shape ng-tns-c3241311687-2']</t>
-  </si>
-  <si>
-    <t>LOGOUT</t>
-  </si>
-  <si>
-    <t>Clicking Account menu in Dashboard</t>
-  </si>
-  <si>
-    <t>//img[@class='logout-user-icon ng-tns-c3241311687-2']</t>
-  </si>
-  <si>
-    <t>Clicking logout button</t>
-  </si>
-  <si>
-    <t>//div[@class='login-header']</t>
-  </si>
-  <si>
-    <t>Back to login page</t>
-  </si>
-  <si>
-    <t>SCROLL</t>
-  </si>
-  <si>
-    <t>Scroll to top</t>
-  </si>
-  <si>
-    <t>Scroll down to bottom</t>
-  </si>
-  <si>
-    <t>SCROLL-TOP</t>
-  </si>
-  <si>
-    <t>SCROLL-BOTTOM</t>
-  </si>
-  <si>
-    <t>Click new application</t>
-  </si>
-  <si>
-    <t>//button[@class='mat-focus-indicator new-application-button mat-button mat-button-base']</t>
-  </si>
-  <si>
-    <t>//*[@id="mat-radio-6"]/label/span[1]/span[2]</t>
-  </si>
-  <si>
-    <t>Select not an applicant patient</t>
-  </si>
-  <si>
-    <t>//img[@src='assets/images/pop-up-close.png']</t>
-  </si>
-  <si>
-    <t>Close new application popup</t>
   </si>
   <si>
     <t>WORKFLOW</t>
@@ -994,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807A929D-612E-412C-BC59-E1482EA51A15}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,330 +922,78 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E5" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D08CDE5-DE8D-42D3-A577-CDBF8B10C916}">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66932E15-50A6-4A7D-8170-FA21EAF8A917}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to send mail
</commit_message>
<xml_diff>
--- a/input/input-file.xlsx
+++ b/input/input-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMV\WS\EWS\jtestng\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDCD16D-9682-46D6-A043-156C60A0E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BB330B-50AA-41C4-B6A5-5C9E4653C2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2AA5BCE-9ACD-4C72-839C-F70134009B4E}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>ACTION</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>EXPECTED</t>
+  </si>
+  <si>
+    <t>STEP_TITLE</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Fill Username</t>
+  </si>
+  <si>
+    <t>Fill Password</t>
+  </si>
+  <si>
+    <t>Submit form</t>
   </si>
 </sst>
 </file>
@@ -902,97 +917,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807A929D-612E-412C-BC59-E1482EA51A15}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>